<commit_message>
Hapus bobot dalam perhtungan
</commit_message>
<xml_diff>
--- a/promethee.xlsx
+++ b/promethee.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XAMPP\htdocs\promethee-ci\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Skripsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A17811-7B72-458E-8AD2-BBCA9D41D873}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="73">
   <si>
     <t>Kriteria</t>
   </si>
@@ -238,15 +239,12 @@
   </si>
   <si>
     <t>Perhitungan Penentuan Alternatif Produk Terbaik dengan Metode PROMETHEE (Preference Ranking Organization Method For Enrichment Evaluation)</t>
-  </si>
-  <si>
-    <t>https://rumahsourcecode.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -675,37 +673,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
         <v>0</v>
       </c>
@@ -729,7 +725,7 @@
       </c>
       <c r="K5" s="24"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -753,7 +749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -785,7 +781,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
@@ -815,7 +811,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
@@ -845,7 +841,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
@@ -875,7 +871,7 @@
       </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
@@ -907,7 +903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
@@ -935,13 +931,13 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D13" s="3">
         <f>SUM(D7:D12)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
@@ -974,7 +970,7 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>26</v>
       </c>
@@ -1016,7 +1012,7 @@
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
         <v>25</v>
       </c>
@@ -1058,7 +1054,7 @@
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>16</v>
       </c>
@@ -1100,7 +1096,7 @@
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
@@ -1142,7 +1138,7 @@
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>58</v>
       </c>
@@ -1184,7 +1180,7 @@
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>29</v>
       </c>
@@ -1226,7 +1222,7 @@
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>36</v>
       </c>
@@ -1268,7 +1264,7 @@
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="D23" s="4" t="s">
         <v>4</v>
@@ -1308,7 +1304,7 @@
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
       <c r="D24" s="4" t="s">
         <v>3</v>
@@ -1348,7 +1344,7 @@
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="D25" s="4" t="s">
         <v>5</v>
@@ -1388,7 +1384,7 @@
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="D26" s="4" t="s">
         <v>4</v>
@@ -1428,7 +1424,7 @@
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="D27" s="4" t="s">
         <v>5</v>
@@ -1468,7 +1464,7 @@
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>10</v>
       </c>
@@ -1501,7 +1497,7 @@
       <c r="P29" s="10"/>
       <c r="Q29" s="10"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="s">
         <v>24</v>
       </c>
@@ -1543,7 +1539,7 @@
       <c r="P30" s="10"/>
       <c r="Q30" s="10"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" s="12" t="s">
         <v>23</v>
       </c>
@@ -1585,7 +1581,7 @@
       <c r="P31" s="10"/>
       <c r="Q31" s="10"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
         <v>17</v>
       </c>
@@ -1627,7 +1623,7 @@
       <c r="P32" s="10"/>
       <c r="Q32" s="10"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
         <v>42</v>
       </c>
@@ -1669,7 +1665,7 @@
       <c r="P33" s="10"/>
       <c r="Q33" s="10"/>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
         <v>43</v>
       </c>
@@ -1711,7 +1707,7 @@
       <c r="P34" s="10"/>
       <c r="Q34" s="10"/>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" s="10" t="s">
         <v>40</v>
       </c>
@@ -1753,7 +1749,7 @@
       <c r="P35" s="10"/>
       <c r="Q35" s="10"/>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36" s="10"/>
       <c r="D36" s="10" t="s">
         <v>3</v>
@@ -1793,7 +1789,7 @@
       <c r="P36" s="10"/>
       <c r="Q36" s="10"/>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" s="10"/>
       <c r="D37" s="10" t="s">
         <v>4</v>
@@ -1833,7 +1829,7 @@
       <c r="P37" s="10"/>
       <c r="Q37" s="10"/>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38" s="10"/>
       <c r="D38" s="10" t="s">
         <v>3</v>
@@ -1873,7 +1869,7 @@
       <c r="P38" s="10"/>
       <c r="Q38" s="10"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" s="10"/>
       <c r="D39" s="10" t="s">
         <v>5</v>
@@ -1913,7 +1909,7 @@
       <c r="P39" s="10"/>
       <c r="Q39" s="10"/>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40" s="10"/>
       <c r="D40" s="10" t="s">
         <v>4</v>
@@ -1953,7 +1949,7 @@
       <c r="P40" s="10"/>
       <c r="Q40" s="10"/>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" s="10"/>
       <c r="D41" s="10" t="s">
         <v>5</v>
@@ -1993,7 +1989,7 @@
       <c r="P41" s="10"/>
       <c r="Q41" s="10"/>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>11</v>
       </c>
@@ -2026,7 +2022,7 @@
       <c r="P43" s="5"/>
       <c r="Q43" s="5"/>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B44" s="14" t="s">
         <v>24</v>
       </c>
@@ -2068,7 +2064,7 @@
       <c r="P44" s="5"/>
       <c r="Q44" s="5"/>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B45" s="15" t="s">
         <v>23</v>
       </c>
@@ -2110,7 +2106,7 @@
       <c r="P45" s="5"/>
       <c r="Q45" s="5"/>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>45</v>
       </c>
@@ -2152,7 +2148,7 @@
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>42</v>
       </c>
@@ -2194,7 +2190,7 @@
       <c r="P47" s="5"/>
       <c r="Q47" s="5"/>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
         <v>43</v>
       </c>
@@ -2236,7 +2232,7 @@
       <c r="P48" s="5"/>
       <c r="Q48" s="5"/>
     </row>
-    <row r="49" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>36</v>
       </c>
@@ -2278,7 +2274,7 @@
       <c r="P49" s="5"/>
       <c r="Q49" s="5"/>
     </row>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B50" s="5"/>
       <c r="D50" s="5" t="s">
         <v>3</v>
@@ -2318,7 +2314,7 @@
       <c r="P50" s="5"/>
       <c r="Q50" s="5"/>
     </row>
-    <row r="51" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B51" s="5"/>
       <c r="D51" s="5" t="s">
         <v>4</v>
@@ -2358,7 +2354,7 @@
       <c r="P51" s="5"/>
       <c r="Q51" s="5"/>
     </row>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
       <c r="D52" s="5" t="s">
         <v>3</v>
@@ -2398,7 +2394,7 @@
       <c r="P52" s="5"/>
       <c r="Q52" s="5"/>
     </row>
-    <row r="53" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B53" s="5"/>
       <c r="D53" s="5" t="s">
         <v>5</v>
@@ -2438,7 +2434,7 @@
       <c r="P53" s="5"/>
       <c r="Q53" s="5"/>
     </row>
-    <row r="54" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
       <c r="D54" s="5" t="s">
         <v>4</v>
@@ -2478,7 +2474,7 @@
       <c r="P54" s="5"/>
       <c r="Q54" s="5"/>
     </row>
-    <row r="55" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
       <c r="D55" s="5" t="s">
         <v>5</v>
@@ -2518,7 +2514,7 @@
       <c r="P55" s="5"/>
       <c r="Q55" s="5"/>
     </row>
-    <row r="57" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B57" s="19" t="s">
         <v>12</v>
       </c>
@@ -2551,7 +2547,7 @@
       <c r="P57" s="19"/>
       <c r="Q57" s="19"/>
     </row>
-    <row r="58" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B58" s="20" t="s">
         <v>52</v>
       </c>
@@ -2593,7 +2589,7 @@
       <c r="P58" s="19"/>
       <c r="Q58" s="19"/>
     </row>
-    <row r="59" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B59" s="21" t="s">
         <v>23</v>
       </c>
@@ -2635,7 +2631,7 @@
       <c r="P59" s="19"/>
       <c r="Q59" s="19"/>
     </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B60" s="19" t="s">
         <v>53</v>
       </c>
@@ -2677,7 +2673,7 @@
       <c r="P60" s="19"/>
       <c r="Q60" s="19"/>
     </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B61" s="19" t="s">
         <v>55</v>
       </c>
@@ -2719,7 +2715,7 @@
       <c r="P61" s="19"/>
       <c r="Q61" s="19"/>
     </row>
-    <row r="62" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B62" s="19" t="s">
         <v>56</v>
       </c>
@@ -2761,7 +2757,7 @@
       <c r="P62" s="19"/>
       <c r="Q62" s="19"/>
     </row>
-    <row r="63" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B63" s="19" t="s">
         <v>48</v>
       </c>
@@ -2803,7 +2799,7 @@
       <c r="P63" s="19"/>
       <c r="Q63" s="19"/>
     </row>
-    <row r="64" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B64" s="19"/>
       <c r="D64" s="19" t="s">
         <v>3</v>
@@ -2843,7 +2839,7 @@
       <c r="P64" s="19"/>
       <c r="Q64" s="19"/>
     </row>
-    <row r="65" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B65" s="19"/>
       <c r="D65" s="19" t="s">
         <v>4</v>
@@ -2883,7 +2879,7 @@
       <c r="P65" s="19"/>
       <c r="Q65" s="19"/>
     </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B66" s="19"/>
       <c r="D66" s="19" t="s">
         <v>3</v>
@@ -2923,7 +2919,7 @@
       <c r="P66" s="19"/>
       <c r="Q66" s="19"/>
     </row>
-    <row r="67" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B67" s="19"/>
       <c r="D67" s="19" t="s">
         <v>5</v>
@@ -2963,7 +2959,7 @@
       <c r="P67" s="19"/>
       <c r="Q67" s="19"/>
     </row>
-    <row r="68" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B68" s="19"/>
       <c r="D68" s="19" t="s">
         <v>4</v>
@@ -3003,7 +2999,7 @@
       <c r="P68" s="19"/>
       <c r="Q68" s="19"/>
     </row>
-    <row r="69" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B69" s="19"/>
       <c r="D69" s="19" t="s">
         <v>5</v>
@@ -3043,7 +3039,7 @@
       <c r="P69" s="19"/>
       <c r="Q69" s="19"/>
     </row>
-    <row r="71" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B71" s="16" t="s">
         <v>13</v>
       </c>
@@ -3076,7 +3072,7 @@
       <c r="P71" s="16"/>
       <c r="Q71" s="16"/>
     </row>
-    <row r="72" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B72" s="17" t="s">
         <v>57</v>
       </c>
@@ -3118,7 +3114,7 @@
       <c r="P72" s="16"/>
       <c r="Q72" s="16"/>
     </row>
-    <row r="73" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B73" s="18" t="s">
         <v>25</v>
       </c>
@@ -3160,7 +3156,7 @@
       <c r="P73" s="16"/>
       <c r="Q73" s="16"/>
     </row>
-    <row r="74" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B74" s="16" t="s">
         <v>59</v>
       </c>
@@ -3202,7 +3198,7 @@
       <c r="P74" s="16"/>
       <c r="Q74" s="16"/>
     </row>
-    <row r="75" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B75" s="16" t="s">
         <v>27</v>
       </c>
@@ -3244,7 +3240,7 @@
       <c r="P75" s="16"/>
       <c r="Q75" s="16"/>
     </row>
-    <row r="76" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B76" s="16" t="s">
         <v>28</v>
       </c>
@@ -3286,7 +3282,7 @@
       <c r="P76" s="16"/>
       <c r="Q76" s="16"/>
     </row>
-    <row r="77" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B77" s="16" t="s">
         <v>29</v>
       </c>
@@ -3328,7 +3324,7 @@
       <c r="P77" s="16"/>
       <c r="Q77" s="16"/>
     </row>
-    <row r="78" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B78" s="16" t="s">
         <v>48</v>
       </c>
@@ -3370,7 +3366,7 @@
       <c r="P78" s="16"/>
       <c r="Q78" s="16"/>
     </row>
-    <row r="79" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B79" s="16"/>
       <c r="D79" s="16" t="s">
         <v>4</v>
@@ -3410,7 +3406,7 @@
       <c r="P79" s="16"/>
       <c r="Q79" s="16"/>
     </row>
-    <row r="80" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B80" s="16"/>
       <c r="D80" s="16" t="s">
         <v>3</v>
@@ -3450,7 +3446,7 @@
       <c r="P80" s="16"/>
       <c r="Q80" s="16"/>
     </row>
-    <row r="81" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B81" s="16"/>
       <c r="D81" s="16" t="s">
         <v>5</v>
@@ -3490,7 +3486,7 @@
       <c r="P81" s="16"/>
       <c r="Q81" s="16"/>
     </row>
-    <row r="82" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B82" s="16"/>
       <c r="D82" s="16" t="s">
         <v>4</v>
@@ -3530,7 +3526,7 @@
       <c r="P82" s="16"/>
       <c r="Q82" s="16"/>
     </row>
-    <row r="83" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B83" s="16"/>
       <c r="D83" s="16" t="s">
         <v>5</v>
@@ -3570,7 +3566,7 @@
       <c r="P83" s="16"/>
       <c r="Q83" s="16"/>
     </row>
-    <row r="85" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B85" s="6" t="s">
         <v>14</v>
       </c>
@@ -3603,7 +3599,7 @@
       <c r="P85" s="6"/>
       <c r="Q85" s="6"/>
     </row>
-    <row r="86" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B86" s="22" t="s">
         <v>47</v>
       </c>
@@ -3645,7 +3641,7 @@
       <c r="P86" s="6"/>
       <c r="Q86" s="6"/>
     </row>
-    <row r="87" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B87" s="23" t="s">
         <v>23</v>
       </c>
@@ -3687,7 +3683,7 @@
       <c r="P87" s="6"/>
       <c r="Q87" s="6"/>
     </row>
-    <row r="88" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B88" s="6" t="s">
         <v>49</v>
       </c>
@@ -3729,7 +3725,7 @@
       <c r="P88" s="6"/>
       <c r="Q88" s="6"/>
     </row>
-    <row r="89" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B89" s="6" t="s">
         <v>50</v>
       </c>
@@ -3771,7 +3767,7 @@
       <c r="P89" s="6"/>
       <c r="Q89" s="6"/>
     </row>
-    <row r="90" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B90" s="6" t="s">
         <v>54</v>
       </c>
@@ -3813,7 +3809,7 @@
       <c r="P90" s="6"/>
       <c r="Q90" s="6"/>
     </row>
-    <row r="91" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B91" s="6"/>
       <c r="D91" s="6" t="s">
         <v>5</v>
@@ -3853,7 +3849,7 @@
       <c r="P91" s="6"/>
       <c r="Q91" s="6"/>
     </row>
-    <row r="92" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B92" s="6"/>
       <c r="D92" s="6" t="s">
         <v>3</v>
@@ -3893,7 +3889,7 @@
       <c r="P92" s="6"/>
       <c r="Q92" s="6"/>
     </row>
-    <row r="93" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B93" s="6"/>
       <c r="D93" s="6" t="s">
         <v>4</v>
@@ -3933,7 +3929,7 @@
       <c r="P93" s="6"/>
       <c r="Q93" s="6"/>
     </row>
-    <row r="94" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B94" s="6"/>
       <c r="D94" s="6" t="s">
         <v>3</v>
@@ -3973,7 +3969,7 @@
       <c r="P94" s="6"/>
       <c r="Q94" s="6"/>
     </row>
-    <row r="95" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B95" s="6"/>
       <c r="D95" s="6" t="s">
         <v>5</v>
@@ -4013,7 +4009,7 @@
       <c r="P95" s="6"/>
       <c r="Q95" s="6"/>
     </row>
-    <row r="96" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B96" s="6"/>
       <c r="D96" s="6" t="s">
         <v>4</v>
@@ -4053,7 +4049,7 @@
       <c r="P96" s="6"/>
       <c r="Q96" s="6"/>
     </row>
-    <row r="97" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B97" s="6"/>
       <c r="D97" s="6" t="s">
         <v>5</v>
@@ -4093,7 +4089,7 @@
       <c r="P97" s="6"/>
       <c r="Q97" s="6"/>
     </row>
-    <row r="101" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D101" s="7" t="s">
         <v>64</v>
       </c>
@@ -4121,7 +4117,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="102" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D102" s="7" t="s">
         <v>2</v>
       </c>
@@ -4159,7 +4155,7 @@
         <v>0.25833333333333336</v>
       </c>
     </row>
-    <row r="103" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D103" s="7" t="s">
         <v>3</v>
       </c>
@@ -4197,7 +4193,7 @@
         <v>0.34166666666666662</v>
       </c>
     </row>
-    <row r="104" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D104" s="7" t="s">
         <v>2</v>
       </c>
@@ -4235,7 +4231,7 @@
         <v>0.31666666666666665</v>
       </c>
     </row>
-    <row r="105" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D105" s="7" t="s">
         <v>4</v>
       </c>
@@ -4273,7 +4269,7 @@
         <v>0.10000000000000002</v>
       </c>
     </row>
-    <row r="106" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D106" s="7" t="s">
         <v>2</v>
       </c>
@@ -4306,7 +4302,7 @@
       <c r="N106" s="19"/>
       <c r="O106" s="19"/>
     </row>
-    <row r="107" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D107" s="7" t="s">
         <v>5</v>
       </c>
@@ -4339,7 +4335,7 @@
       <c r="N107" s="19"/>
       <c r="O107" s="19"/>
     </row>
-    <row r="108" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D108" s="7" t="s">
         <v>3</v>
       </c>
@@ -4351,7 +4347,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="109" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D109" s="7" t="s">
         <v>4</v>
       </c>
@@ -4378,7 +4374,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="110" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D110" s="7" t="s">
         <v>3</v>
       </c>
@@ -4408,7 +4404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D111" s="7" t="s">
         <v>5</v>
       </c>
@@ -4438,7 +4434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D112" s="7" t="s">
         <v>4</v>
       </c>
@@ -4468,7 +4464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="113" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D113" s="7" t="s">
         <v>5</v>
       </c>
@@ -4507,10 +4503,7 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="I5:I6"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>